<commit_message>
Infos Update about new version
</commit_message>
<xml_diff>
--- a/docs/NewStatistics_result.xlsx
+++ b/docs/NewStatistics_result.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes_OpenSource\Karstnet_CHYNRepo\karstnet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07220E3-D46E-4429-A2E1-1D7CC531B6EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54122DC7-FEEE-4205-A510-CE7F72B26820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="435" windowWidth="31755" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompleteResults" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -292,9 +295,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,6 +314,177 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="AvecDonneespreserv"/>
+      <sheetName val="Extraits_Karstnet"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="H2">
+            <v>0.96391323198532708</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="H3">
+            <v>0.91795668523140161</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="H4">
+            <v>0.90684390955960203</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="H6">
+            <v>0.97170725722511009</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="H7">
+            <v>0.98614046849145764</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="H8">
+            <v>0.74573539744309381</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="H9">
+            <v>0.89229037428228086</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="H12">
+            <v>0.92122082359284563</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="H13">
+            <v>0.94747793012154657</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="H14">
+            <v>0.92751201633178659</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="H15">
+            <v>0.98699309568257187</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="H16">
+            <v>0.88432458256038959</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="H17">
+            <v>0.9808993416742583</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="H18">
+            <v>0.97564721766630569</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="H19">
+            <v>0.99616280072638397</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="H20">
+            <v>0.99590958062321266</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="H21">
+            <v>0.95387520990238139</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="H22">
+            <v>0.99586013950525853</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="H23">
+            <v>0.98376120871469575</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="H24">
+            <v>0.96394070160922196</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="H25">
+            <v>0.99699369719480535</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="H26">
+            <v>0.93271111702492882</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="H27">
+            <v>0.98604301406962025</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="H28">
+            <v>0.99247128241993354</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="H29">
+            <v>0.99240044947702777</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="H30">
+            <v>0.98779620186933115</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="H31">
+            <v>0.98784789210726376</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="H32">
+            <v>0.97812149727693598</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="H33">
+            <v>0.99131000833124872</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="H34">
+            <v>0.99098552042888643</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="H35">
+            <v>0.98244681613567253</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,7 +811,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,14 +898,15 @@
       <c r="C2" s="8">
         <v>1893</v>
       </c>
-      <c r="D2" s="9">
-        <v>0.95874881007622381</v>
+      <c r="D2" s="11">
+        <f>[1]Extraits_Karstnet!H2</f>
+        <v>0.96391323198532708</v>
       </c>
       <c r="E2" s="4">
         <v>113.41601042609081</v>
       </c>
       <c r="F2" s="4">
-        <v>0.28236564451602569</v>
+        <v>0.29399874834163608</v>
       </c>
       <c r="G2" s="5">
         <v>1.89213462302246</v>
@@ -751,19 +926,19 @@
       <c r="L2" s="4">
         <v>20</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <v>7.9100000000000004E-3</v>
       </c>
       <c r="N2" s="8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="O2" s="10">
+      <c r="O2" s="9">
         <v>3.8850000000000003E-2</v>
       </c>
       <c r="P2" s="8">
         <v>31.82</v>
       </c>
-      <c r="Q2" s="10">
+      <c r="Q2" s="9">
         <v>5.7000000000000002E-3</v>
       </c>
       <c r="R2" s="4">
@@ -793,14 +968,15 @@
       <c r="C3" s="8">
         <v>1477</v>
       </c>
-      <c r="D3" s="9">
-        <v>0.90765078703075452</v>
+      <c r="D3" s="11">
+        <f>[1]Extraits_Karstnet!H3</f>
+        <v>0.91795668523140161</v>
       </c>
       <c r="E3" s="4">
         <v>70.730479372288627</v>
       </c>
       <c r="F3" s="4">
-        <v>0.48700026492934873</v>
+        <v>0.54279602893966661</v>
       </c>
       <c r="G3" s="5">
         <v>1.088098158223445</v>
@@ -820,19 +996,19 @@
       <c r="L3" s="4">
         <v>18</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <v>5.0700000000000007E-3</v>
       </c>
       <c r="N3" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="P3" s="8">
         <v>19.95</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="9">
         <v>4.0199999999999993E-3</v>
       </c>
       <c r="R3" s="4">
@@ -862,14 +1038,15 @@
       <c r="C4" s="8">
         <v>6268</v>
       </c>
-      <c r="D4" s="9">
-        <v>0.89938678693097618</v>
+      <c r="D4" s="11">
+        <f>[1]Extraits_Karstnet!H4</f>
+        <v>0.90684390955960203</v>
       </c>
       <c r="E4" s="4">
         <v>69.736108997415826</v>
       </c>
       <c r="F4" s="4">
-        <v>0.20506701842209049</v>
+        <v>0.2124312142965456</v>
       </c>
       <c r="G4" s="5">
         <v>1.492467810247597</v>
@@ -889,19 +1066,19 @@
       <c r="L4" s="4">
         <v>14</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="N4" s="8">
         <v>1.01</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <v>3.3829999999999999E-2</v>
       </c>
       <c r="P4" s="8">
         <v>3.52</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="9">
         <v>8.3000000000000001E-4</v>
       </c>
       <c r="R4" s="4">
@@ -950,19 +1127,19 @@
       <c r="L5" s="4">
         <v>27</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>2.8500000000000001E-3</v>
       </c>
       <c r="N5" s="8">
         <v>1.05</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <v>3.5299999999999998E-2</v>
       </c>
       <c r="P5" s="8">
         <v>11.93</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="9">
         <v>2E-3</v>
       </c>
       <c r="R5" s="4">
@@ -992,14 +1169,15 @@
       <c r="C6" s="8">
         <v>886</v>
       </c>
-      <c r="D6" s="9">
-        <v>0.97200015641462356</v>
+      <c r="D6" s="11">
+        <f>[1]Extraits_Karstnet!H6</f>
+        <v>0.97170725722511009</v>
       </c>
       <c r="E6" s="4">
         <v>55.612542486748787</v>
       </c>
       <c r="F6" s="4">
-        <v>0.31013010516355199</v>
+        <v>0.39337986286061349</v>
       </c>
       <c r="G6" s="5">
         <v>1.350763885412007</v>
@@ -1019,19 +1197,19 @@
       <c r="L6" s="4">
         <v>9</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>3.4700000000000004E-3</v>
       </c>
       <c r="N6" s="8">
         <v>1.04</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>3.5130000000000002E-2</v>
       </c>
       <c r="P6" s="8">
         <v>11.33</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="9">
         <v>3.2799999999999999E-3</v>
       </c>
       <c r="R6" s="4">
@@ -1061,14 +1239,15 @@
       <c r="C7" s="8">
         <v>2013</v>
       </c>
-      <c r="D7" s="9">
-        <v>0.98430942907616481</v>
+      <c r="D7" s="11">
+        <f>[1]Extraits_Karstnet!H7</f>
+        <v>0.98614046849145764</v>
       </c>
       <c r="E7" s="4">
         <v>50.840930018601952</v>
       </c>
       <c r="F7" s="4">
-        <v>9.364017471834736E-2</v>
+        <v>0.10122118751514481</v>
       </c>
       <c r="G7" s="5">
         <v>2.5598056682824368</v>
@@ -1088,19 +1267,19 @@
       <c r="L7" s="4">
         <v>29</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>5.6299999999999996E-3</v>
       </c>
       <c r="N7" s="8">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>3.721E-2</v>
       </c>
       <c r="P7" s="8">
         <v>22.94</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="9">
         <v>5.1700000000000001E-3</v>
       </c>
       <c r="R7" s="4">
@@ -1130,14 +1309,15 @@
       <c r="C8" s="8">
         <v>229</v>
       </c>
-      <c r="D8" s="9">
-        <v>0.70881776521222373</v>
+      <c r="D8" s="11">
+        <f>[1]Extraits_Karstnet!H8</f>
+        <v>0.74573539744309381</v>
       </c>
       <c r="E8" s="4">
         <v>331.73526133772009</v>
       </c>
       <c r="F8" s="4">
-        <v>0.5744174271404584</v>
+        <v>0.50106375925542113</v>
       </c>
       <c r="G8" s="5">
         <v>1.5692899322733911</v>
@@ -1157,19 +1337,19 @@
       <c r="L8" s="4">
         <v>0</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <v>0</v>
       </c>
       <c r="N8" s="8">
         <v>0.88</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>3.8890000000000001E-2</v>
       </c>
       <c r="P8" s="8">
         <v>3.21</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="9">
         <v>0</v>
       </c>
       <c r="R8" s="4">
@@ -1199,14 +1379,15 @@
       <c r="C9" s="8">
         <v>146</v>
       </c>
-      <c r="D9" s="9">
-        <v>0.88410071624715814</v>
+      <c r="D9" s="11">
+        <f>[1]Extraits_Karstnet!H9</f>
+        <v>0.89229037428228086</v>
       </c>
       <c r="E9" s="4">
         <v>50.803424363916641</v>
       </c>
       <c r="F9" s="4">
-        <v>0.42024317197569672</v>
+        <v>0.41494542125754891</v>
       </c>
       <c r="G9" s="5">
         <v>1.573141789213131</v>
@@ -1226,19 +1407,19 @@
       <c r="L9" s="4">
         <v>2</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="9">
         <v>6.0599999999999994E-3</v>
       </c>
       <c r="N9" s="8">
         <v>1.05</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>3.9219999999999998E-2</v>
       </c>
       <c r="P9" s="8">
         <v>23.78</v>
       </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="9">
         <v>5.2599999999999999E-3</v>
       </c>
       <c r="R9" s="4">
@@ -1287,19 +1468,19 @@
       <c r="L10" s="4">
         <v>10</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>2E-3</v>
       </c>
       <c r="N10" s="8">
         <v>1.04</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>3.4790000000000001E-2</v>
       </c>
       <c r="P10" s="8">
         <v>8.5500000000000007</v>
       </c>
-      <c r="Q10" s="10">
+      <c r="Q10" s="9">
         <v>1.5500000000000002E-3</v>
       </c>
       <c r="R10" s="4">
@@ -1348,19 +1529,19 @@
       <c r="L11" s="4">
         <v>60</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>8.1400000000000014E-3</v>
       </c>
       <c r="N11" s="8">
         <v>1.1599999999999999</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>3.8840000000000006E-2</v>
       </c>
       <c r="P11" s="8">
         <v>32.92</v>
       </c>
-      <c r="Q11" s="10">
+      <c r="Q11" s="9">
         <v>5.9100000000000003E-3</v>
       </c>
       <c r="R11" s="4">
@@ -1390,14 +1571,15 @@
       <c r="C12" s="8">
         <v>2687</v>
       </c>
-      <c r="D12" s="9">
-        <v>0.91506978493227875</v>
+      <c r="D12" s="11">
+        <f>[1]Extraits_Karstnet!H12</f>
+        <v>0.92122082359284563</v>
       </c>
       <c r="E12" s="4">
         <v>55.663986260028388</v>
       </c>
       <c r="F12" s="4">
-        <v>0.19038157486226839</v>
+        <v>0.20512264458775001</v>
       </c>
       <c r="G12" s="5">
         <v>1.873754306185289</v>
@@ -1417,19 +1599,19 @@
       <c r="L12" s="4">
         <v>23</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="9">
         <v>3.3E-3</v>
       </c>
       <c r="N12" s="8">
         <v>1.06</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>3.5630000000000002E-2</v>
       </c>
       <c r="P12" s="8">
         <v>13.73</v>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="9">
         <v>2.1900000000000001E-3</v>
       </c>
       <c r="R12" s="4">
@@ -1459,14 +1641,15 @@
       <c r="C13" s="8">
         <v>308</v>
       </c>
-      <c r="D13" s="9">
-        <v>0.95270762820224519</v>
+      <c r="D13" s="11">
+        <f>[1]Extraits_Karstnet!H13</f>
+        <v>0.94747793012154657</v>
       </c>
       <c r="E13" s="4">
         <v>15.806543488250909</v>
       </c>
       <c r="F13" s="4">
-        <v>0.49575790336662828</v>
+        <v>0.5742023642120363</v>
       </c>
       <c r="G13" s="5">
         <v>1.293556176526597</v>
@@ -1486,19 +1669,19 @@
       <c r="L13" s="4">
         <v>2</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="9">
         <v>1.17E-3</v>
       </c>
       <c r="N13" s="8">
         <v>1.01</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>3.4500000000000003E-2</v>
       </c>
       <c r="P13" s="8">
         <v>5.25</v>
       </c>
-      <c r="Q13" s="10">
+      <c r="Q13" s="9">
         <v>6.0999999999999997E-4</v>
       </c>
       <c r="R13" s="4">
@@ -1528,14 +1711,15 @@
       <c r="C14" s="8">
         <v>339</v>
       </c>
-      <c r="D14" s="9">
-        <v>0.92037601293801607</v>
+      <c r="D14" s="11">
+        <f>[1]Extraits_Karstnet!H14</f>
+        <v>0.92751201633178659</v>
       </c>
       <c r="E14" s="4">
         <v>33.200309139125352</v>
       </c>
       <c r="F14" s="4">
-        <v>0.27666963436844039</v>
+        <v>0.34570680816175181</v>
       </c>
       <c r="G14" s="5">
         <v>1.614801204244976</v>
@@ -1555,19 +1739,19 @@
       <c r="L14" s="4">
         <v>7</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <v>4.8300000000000001E-3</v>
       </c>
       <c r="N14" s="8">
         <v>1.08</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>3.6990000000000002E-2</v>
       </c>
       <c r="P14" s="8">
         <v>19.59</v>
       </c>
-      <c r="Q14" s="10">
+      <c r="Q14" s="9">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="R14" s="4">
@@ -1597,14 +1781,15 @@
       <c r="C15" s="8">
         <v>2354</v>
       </c>
-      <c r="D15" s="9">
-        <v>0.98622622097149748</v>
+      <c r="D15" s="11">
+        <f>[1]Extraits_Karstnet!H15</f>
+        <v>0.98699309568257187</v>
       </c>
       <c r="E15" s="4">
         <v>62.294731375662273</v>
       </c>
       <c r="F15" s="4">
-        <v>0.51860148580396315</v>
+        <v>0.54267279398540946</v>
       </c>
       <c r="G15" s="5">
         <v>1.4109484687139009</v>
@@ -1624,19 +1809,19 @@
       <c r="L15" s="4">
         <v>29</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>4.8399999999999997E-3</v>
       </c>
       <c r="N15" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="O15" s="10">
+      <c r="O15" s="9">
         <v>3.6670000000000001E-2</v>
       </c>
       <c r="P15" s="8">
         <v>19.829999999999998</v>
       </c>
-      <c r="Q15" s="10">
+      <c r="Q15" s="9">
         <v>3.79E-3</v>
       </c>
       <c r="R15" s="4">
@@ -1666,14 +1851,15 @@
       <c r="C16" s="8">
         <v>163</v>
       </c>
-      <c r="D16" s="9">
-        <v>0.86170854054262425</v>
+      <c r="D16" s="11">
+        <f>[1]Extraits_Karstnet!H16</f>
+        <v>0.88432458256038959</v>
       </c>
       <c r="E16" s="4">
         <v>194.02951080220501</v>
       </c>
-      <c r="F16" s="11">
-        <v>0.69363786366940527</v>
+      <c r="F16" s="10">
+        <v>0.66739008869332295</v>
       </c>
       <c r="G16" s="5">
         <v>0.96570507741674227</v>
@@ -1693,19 +1879,19 @@
       <c r="L16" s="4">
         <v>0</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <v>0</v>
       </c>
       <c r="N16" s="8">
         <v>0.93</v>
       </c>
-      <c r="O16" s="10">
+      <c r="O16" s="9">
         <v>3.5900000000000001E-2</v>
       </c>
       <c r="P16" s="8">
         <v>1.24</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="9">
         <v>0</v>
       </c>
       <c r="R16" s="4">
@@ -1735,14 +1921,15 @@
       <c r="C17" s="8">
         <v>733</v>
       </c>
-      <c r="D17" s="9">
-        <v>0.9733552271157091</v>
+      <c r="D17" s="11">
+        <f>[1]Extraits_Karstnet!H17</f>
+        <v>0.9808993416742583</v>
       </c>
       <c r="E17" s="4">
         <v>29.756566050967159</v>
       </c>
       <c r="F17" s="4">
-        <v>0.54921146491714645</v>
+        <v>0.60692418733150422</v>
       </c>
       <c r="G17" s="5">
         <v>1.0993590314796211</v>
@@ -1762,19 +1949,19 @@
       <c r="L17" s="4">
         <v>11</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="9">
         <v>4.5300000000000002E-3</v>
       </c>
       <c r="N17" s="8">
         <v>1.07</v>
       </c>
-      <c r="O17" s="10">
+      <c r="O17" s="9">
         <v>3.6340000000000004E-2</v>
       </c>
       <c r="P17" s="8">
         <v>17.420000000000002</v>
       </c>
-      <c r="Q17" s="10">
+      <c r="Q17" s="9">
         <v>3.5800000000000003E-3</v>
       </c>
       <c r="R17" s="4">
@@ -1804,14 +1991,15 @@
       <c r="C18" s="8">
         <v>1705</v>
       </c>
-      <c r="D18" s="9">
-        <v>0.98446943022963596</v>
+      <c r="D18" s="11">
+        <f>[1]Extraits_Karstnet!H18</f>
+        <v>0.97564721766630569</v>
       </c>
       <c r="E18" s="4">
         <v>62.057584492336971</v>
       </c>
       <c r="F18" s="4">
-        <v>0.49829745609422571</v>
+        <v>0.5284311689004032</v>
       </c>
       <c r="G18" s="5">
         <v>1.25828219220972</v>
@@ -1831,19 +2019,19 @@
       <c r="L18" s="4">
         <v>40</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="N18" s="8">
         <v>1.28</v>
       </c>
-      <c r="O18" s="10">
+      <c r="O18" s="9">
         <v>4.3490000000000001E-2</v>
       </c>
       <c r="P18" s="8">
         <v>60.46</v>
       </c>
-      <c r="Q18" s="10">
+      <c r="Q18" s="9">
         <v>1.2400000000000001E-2</v>
       </c>
       <c r="R18" s="4">
@@ -1873,14 +2061,15 @@
       <c r="C19" s="8">
         <v>2157</v>
       </c>
-      <c r="D19" s="9">
-        <v>0.99667097158321682</v>
+      <c r="D19" s="11">
+        <f>[1]Extraits_Karstnet!H19</f>
+        <v>0.99616280072638397</v>
       </c>
       <c r="E19" s="4">
         <v>55.835648622191641</v>
       </c>
       <c r="F19" s="4">
-        <v>0.28138748487504073</v>
+        <v>0.32400427763611028</v>
       </c>
       <c r="G19" s="5">
         <v>1.853219904587458</v>
@@ -1900,19 +2089,19 @@
       <c r="L19" s="4">
         <v>8</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="9">
         <v>1.72E-3</v>
       </c>
       <c r="N19" s="8">
         <v>1.03</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="9">
         <v>3.4619999999999998E-2</v>
       </c>
       <c r="P19" s="8">
         <v>7.46</v>
       </c>
-      <c r="Q19" s="10">
+      <c r="Q19" s="9">
         <v>1.1200000000000001E-3</v>
       </c>
       <c r="R19" s="4">
@@ -1942,14 +2131,15 @@
       <c r="C20" s="8">
         <v>13503</v>
       </c>
-      <c r="D20" s="9">
-        <v>0.99539940239875113</v>
+      <c r="D20" s="11">
+        <f>[1]Extraits_Karstnet!H20</f>
+        <v>0.99590958062321266</v>
       </c>
       <c r="E20" s="4">
         <v>69.278278081161588</v>
       </c>
       <c r="F20" s="4">
-        <v>0.44695924218111249</v>
+        <v>0.41439808607474837</v>
       </c>
       <c r="G20" s="5">
         <v>0.9204932820097288</v>
@@ -1969,19 +2159,19 @@
       <c r="L20" s="4">
         <v>779</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>9.3100000000000006E-3</v>
       </c>
       <c r="N20" s="8">
         <v>1.19</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>3.9549999999999995E-2</v>
       </c>
       <c r="P20" s="8">
         <v>37.630000000000003</v>
       </c>
-      <c r="Q20" s="10">
+      <c r="Q20" s="9">
         <v>6.2599999999999999E-3</v>
       </c>
       <c r="R20" s="4">
@@ -2011,14 +2201,15 @@
       <c r="C21" s="8">
         <v>228</v>
       </c>
-      <c r="D21" s="9">
-        <v>0.95177591519613325</v>
+      <c r="D21" s="11">
+        <f>[1]Extraits_Karstnet!H21</f>
+        <v>0.95387520990238139</v>
       </c>
       <c r="E21" s="4">
         <v>15.317507507207919</v>
       </c>
       <c r="F21" s="4">
-        <v>0.46559004461254228</v>
+        <v>0.58208018983087551</v>
       </c>
       <c r="G21" s="5">
         <v>1.1441471475613609</v>
@@ -2038,19 +2229,19 @@
       <c r="L21" s="4">
         <v>1</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="9">
         <v>7.8000000000000009E-4</v>
       </c>
       <c r="N21" s="8">
         <v>0.94</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="9">
         <v>3.2310000000000005E-2</v>
       </c>
       <c r="P21" s="8">
         <v>-4.3</v>
       </c>
-      <c r="Q21" s="10">
+      <c r="Q21" s="9">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R21" s="4">
@@ -2080,14 +2271,15 @@
       <c r="C22" s="8">
         <v>9712</v>
       </c>
-      <c r="D22" s="9">
-        <v>0.99621929781677598</v>
+      <c r="D22" s="11">
+        <f>[1]Extraits_Karstnet!H22</f>
+        <v>0.99586013950525853</v>
       </c>
       <c r="E22" s="4">
         <v>30.598779651685771</v>
       </c>
       <c r="F22" s="4">
-        <v>0.1302166783094473</v>
+        <v>0.1164735567600836</v>
       </c>
       <c r="G22" s="5">
         <v>1.274938379103135</v>
@@ -2107,19 +2299,19 @@
       <c r="L22" s="4">
         <v>389</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <v>8.9800000000000001E-3</v>
       </c>
       <c r="N22" s="8">
         <v>1.17</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="9">
         <v>3.8969999999999998E-2</v>
       </c>
       <c r="P22" s="8">
         <v>34.869999999999997</v>
       </c>
-      <c r="Q22" s="10">
+      <c r="Q22" s="9">
         <v>6.4400000000000004E-3</v>
       </c>
       <c r="R22" s="4">
@@ -2149,14 +2341,15 @@
       <c r="C23" s="8">
         <v>258</v>
       </c>
-      <c r="D23" s="9">
-        <v>0.97979631585699667</v>
+      <c r="D23" s="11">
+        <f>[1]Extraits_Karstnet!H23</f>
+        <v>0.98376120871469575</v>
       </c>
       <c r="E23" s="4">
         <v>8.4641155728075272</v>
       </c>
       <c r="F23" s="4">
-        <v>0.50209478463010326</v>
+        <v>0.55102314306876621</v>
       </c>
       <c r="G23" s="5">
         <v>0.90328817667534111</v>
@@ -2176,19 +2369,19 @@
       <c r="L23" s="4">
         <v>8</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <v>5.1600000000000005E-3</v>
       </c>
       <c r="N23" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="O23" s="10">
+      <c r="O23" s="9">
         <v>3.7179999999999998E-2</v>
       </c>
       <c r="P23" s="8">
         <v>20.91</v>
       </c>
-      <c r="Q23" s="10">
+      <c r="Q23" s="9">
         <v>3.63E-3</v>
       </c>
       <c r="R23" s="4">
@@ -2218,14 +2411,15 @@
       <c r="C24" s="8">
         <v>1326</v>
       </c>
-      <c r="D24" s="9">
-        <v>0.96044507988384753</v>
+      <c r="D24" s="11">
+        <f>[1]Extraits_Karstnet!H24</f>
+        <v>0.96394070160922196</v>
       </c>
       <c r="E24" s="4">
         <v>43.812659729707299</v>
       </c>
       <c r="F24" s="4">
-        <v>0.35781048129688448</v>
+        <v>0.39768160531749058</v>
       </c>
       <c r="G24" s="5">
         <v>1.4267236228508891</v>
@@ -2245,19 +2439,19 @@
       <c r="L24" s="4">
         <v>35</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <v>6.8500000000000002E-3</v>
       </c>
       <c r="N24" s="8">
         <v>1.1299999999999999</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O24" s="9">
         <v>3.8020000000000005E-2</v>
       </c>
       <c r="P24" s="8">
         <v>27.76</v>
       </c>
-      <c r="Q24" s="10">
+      <c r="Q24" s="9">
         <v>5.0999999999999995E-3</v>
       </c>
       <c r="R24" s="4">
@@ -2287,14 +2481,15 @@
       <c r="C25" s="8">
         <v>10098</v>
       </c>
-      <c r="D25" s="9">
-        <v>0.99733481220387976</v>
+      <c r="D25" s="11">
+        <f>[1]Extraits_Karstnet!H25</f>
+        <v>0.99699369719480535</v>
       </c>
       <c r="E25" s="4">
         <v>170.79423192975821</v>
       </c>
       <c r="F25" s="4">
-        <v>0.55231207670552662</v>
+        <v>0.57000955191122882</v>
       </c>
       <c r="G25" s="5">
         <v>0.94022725679586205</v>
@@ -2314,19 +2509,19 @@
       <c r="L25" s="4">
         <v>1</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="9">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="N25" s="8">
         <v>1</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="9">
         <v>3.3409999999999995E-2</v>
       </c>
       <c r="P25" s="8">
         <v>0.89</v>
       </c>
-      <c r="Q25" s="10">
+      <c r="Q25" s="9">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="R25" s="4">
@@ -2356,14 +2551,15 @@
       <c r="C26" s="8">
         <v>309</v>
       </c>
-      <c r="D26" s="9">
-        <v>0.96159405305994339</v>
+      <c r="D26" s="11">
+        <f>[1]Extraits_Karstnet!H26</f>
+        <v>0.93271111702492882</v>
       </c>
       <c r="E26" s="4">
         <v>25.509351166054909</v>
       </c>
       <c r="F26" s="4">
-        <v>0.4253384648639788</v>
+        <v>0.59830217857369261</v>
       </c>
       <c r="G26" s="5">
         <v>1.13555586332081</v>
@@ -2383,19 +2579,19 @@
       <c r="L26" s="4">
         <v>18</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26" s="9">
         <v>2.1299999999999999E-3</v>
       </c>
       <c r="N26" s="8">
         <v>1</v>
       </c>
-      <c r="O26" s="10">
+      <c r="O26" s="9">
         <v>3.6110000000000003E-2</v>
       </c>
       <c r="P26" s="8">
         <v>7.58</v>
       </c>
-      <c r="Q26" s="10">
+      <c r="Q26" s="9">
         <v>2.5600000000000002E-3</v>
       </c>
       <c r="R26" s="4">
@@ -2425,14 +2621,15 @@
       <c r="C27" s="8">
         <v>693</v>
       </c>
-      <c r="D27" s="9">
-        <v>0.98423699894744088</v>
+      <c r="D27" s="11">
+        <f>[1]Extraits_Karstnet!H27</f>
+        <v>0.98604301406962025</v>
       </c>
       <c r="E27" s="4">
         <v>64.267227997869895</v>
       </c>
       <c r="F27" s="4">
-        <v>0.15287727274173141</v>
+        <v>0.33451439799842658</v>
       </c>
       <c r="G27" s="5">
         <v>1.5957167369452081</v>
@@ -2452,19 +2649,19 @@
       <c r="L27" s="4">
         <v>2</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="9">
         <v>1.7700000000000001E-3</v>
       </c>
       <c r="N27" s="8">
         <v>1.02</v>
       </c>
-      <c r="O27" s="10">
+      <c r="O27" s="9">
         <v>3.5090000000000003E-2</v>
       </c>
       <c r="P27" s="8">
         <v>7.58</v>
       </c>
-      <c r="Q27" s="10">
+      <c r="Q27" s="9">
         <v>1.1299999999999999E-3</v>
       </c>
       <c r="R27" s="4">
@@ -2494,14 +2691,15 @@
       <c r="C28" s="8">
         <v>5556</v>
       </c>
-      <c r="D28" s="9">
-        <v>0.99133868728534968</v>
+      <c r="D28" s="11">
+        <f>[1]Extraits_Karstnet!H28</f>
+        <v>0.99247128241993354</v>
       </c>
       <c r="E28" s="4">
         <v>76.103925340074284</v>
       </c>
       <c r="F28" s="4">
-        <v>0.28045926339815258</v>
+        <v>0.28658795601491333</v>
       </c>
       <c r="G28" s="5">
         <v>1.7703910133054239</v>
@@ -2521,19 +2719,19 @@
       <c r="L28" s="4">
         <v>53</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28" s="9">
         <v>3.7300000000000002E-3</v>
       </c>
       <c r="N28" s="8">
         <v>1.07</v>
       </c>
-      <c r="O28" s="10">
+      <c r="O28" s="9">
         <v>3.5770000000000003E-2</v>
       </c>
       <c r="P28" s="8">
         <v>15.08</v>
       </c>
-      <c r="Q28" s="10">
+      <c r="Q28" s="9">
         <v>2.8300000000000001E-3</v>
       </c>
       <c r="R28" s="4">
@@ -2563,14 +2761,15 @@
       <c r="C29" s="8">
         <v>1784</v>
       </c>
-      <c r="D29" s="9">
-        <v>0.99297387636533863</v>
+      <c r="D29" s="11">
+        <f>[1]Extraits_Karstnet!H29</f>
+        <v>0.99240044947702777</v>
       </c>
       <c r="E29" s="4">
         <v>20.705914308268749</v>
       </c>
       <c r="F29" s="4">
-        <v>0.34458941010949051</v>
+        <v>0.37703719294691329</v>
       </c>
       <c r="G29" s="5">
         <v>0.91491869803328996</v>
@@ -2590,19 +2789,19 @@
       <c r="L29" s="4">
         <v>69</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="9">
         <v>1.01E-2</v>
       </c>
       <c r="N29" s="8">
         <v>1.2</v>
       </c>
-      <c r="O29" s="10">
+      <c r="O29" s="9">
         <v>4.0159999999999994E-2</v>
       </c>
       <c r="P29" s="8">
         <v>40.68</v>
       </c>
-      <c r="Q29" s="10">
+      <c r="Q29" s="9">
         <v>6.4600000000000005E-3</v>
       </c>
       <c r="R29" s="4">
@@ -2632,14 +2831,15 @@
       <c r="C30" s="8">
         <v>7634</v>
       </c>
-      <c r="D30" s="9">
-        <v>0.98606742643832779</v>
+      <c r="D30" s="11">
+        <f>[1]Extraits_Karstnet!H30</f>
+        <v>0.98779620186933115</v>
       </c>
       <c r="E30" s="4">
         <v>118.7004705905793</v>
       </c>
       <c r="F30" s="4">
-        <v>0.31982673048142352</v>
+        <v>0.31036882572673602</v>
       </c>
       <c r="G30" s="5">
         <v>1.2780222131295429</v>
@@ -2659,19 +2859,19 @@
       <c r="L30" s="4">
         <v>56</v>
       </c>
-      <c r="M30" s="10">
+      <c r="M30" s="9">
         <v>2.65E-3</v>
       </c>
       <c r="N30" s="8">
         <v>1.05</v>
       </c>
-      <c r="O30" s="10">
+      <c r="O30" s="9">
         <v>3.5070000000000004E-2</v>
       </c>
       <c r="P30" s="8">
         <v>10.93</v>
       </c>
-      <c r="Q30" s="10">
+      <c r="Q30" s="9">
         <v>1.91E-3</v>
       </c>
       <c r="R30" s="4">
@@ -2701,14 +2901,15 @@
       <c r="C31" s="8">
         <v>15570</v>
       </c>
-      <c r="D31" s="9">
-        <v>0.98852445161338431</v>
+      <c r="D31" s="11">
+        <f>[1]Extraits_Karstnet!H31</f>
+        <v>0.98784789210726376</v>
       </c>
       <c r="E31" s="4">
         <v>36.828321050046192</v>
       </c>
-      <c r="F31" s="11">
-        <v>8.6123893988158978E-2</v>
+      <c r="F31" s="10">
+        <v>7.0053569373564994E-2</v>
       </c>
       <c r="G31" s="5">
         <v>1.7276946547799561</v>
@@ -2728,19 +2929,19 @@
       <c r="L31" s="4">
         <v>231</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31" s="9">
         <v>5.6100000000000004E-3</v>
       </c>
       <c r="N31" s="8">
         <v>1.1100000000000001</v>
       </c>
-      <c r="O31" s="10">
+      <c r="O31" s="9">
         <v>3.7090000000000005E-2</v>
       </c>
       <c r="P31" s="8">
         <v>22.92</v>
       </c>
-      <c r="Q31" s="10">
+      <c r="Q31" s="9">
         <v>4.3400000000000001E-3</v>
       </c>
       <c r="R31" s="4">
@@ -2770,14 +2971,15 @@
       <c r="C32" s="8">
         <v>753</v>
       </c>
-      <c r="D32" s="9">
-        <v>0.97358579317346361</v>
+      <c r="D32" s="11">
+        <f>[1]Extraits_Karstnet!H32</f>
+        <v>0.97812149727693598</v>
       </c>
       <c r="E32" s="4">
         <v>52.460223273716473</v>
       </c>
       <c r="F32" s="4">
-        <v>0.597668882125729</v>
+        <v>0.65198943768601392</v>
       </c>
       <c r="G32" s="5">
         <v>1.0399062160951349</v>
@@ -2797,19 +2999,19 @@
       <c r="L32" s="4">
         <v>5</v>
       </c>
-      <c r="M32" s="10">
+      <c r="M32" s="9">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="N32" s="8">
         <v>1</v>
       </c>
-      <c r="O32" s="10">
+      <c r="O32" s="9">
         <v>3.4390000000000004E-2</v>
       </c>
       <c r="P32" s="8">
         <v>8.06</v>
       </c>
-      <c r="Q32" s="10">
+      <c r="Q32" s="9">
         <v>3.2400000000000003E-3</v>
       </c>
       <c r="R32" s="4">
@@ -2839,14 +3041,15 @@
       <c r="C33" s="8">
         <v>1915</v>
       </c>
-      <c r="D33" s="9">
-        <v>0.98875805078364609</v>
+      <c r="D33" s="11">
+        <f>[1]Extraits_Karstnet!H33</f>
+        <v>0.99131000833124872</v>
       </c>
       <c r="E33" s="4">
         <v>26.97188007138968</v>
       </c>
       <c r="F33" s="4">
-        <v>0.42370426758674279</v>
+        <v>0.45035372415828379</v>
       </c>
       <c r="G33" s="5">
         <v>1.322167596472821</v>
@@ -2866,19 +3069,19 @@
       <c r="L33" s="4">
         <v>35</v>
       </c>
-      <c r="M33" s="10">
+      <c r="M33" s="9">
         <v>7.0700000000000008E-3</v>
       </c>
       <c r="N33" s="8">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O33" s="10">
+      <c r="O33" s="9">
         <v>3.8170000000000003E-2</v>
       </c>
       <c r="P33" s="8">
         <v>28.64</v>
       </c>
-      <c r="Q33" s="10">
+      <c r="Q33" s="9">
         <v>5.2400000000000007E-3</v>
       </c>
       <c r="R33" s="4">
@@ -2908,14 +3111,15 @@
       <c r="C34" s="8">
         <v>1418</v>
       </c>
-      <c r="D34" s="9">
-        <v>0.99186672302999312</v>
+      <c r="D34" s="11">
+        <f>[1]Extraits_Karstnet!H34</f>
+        <v>0.99098552042888643</v>
       </c>
       <c r="E34" s="4">
         <v>39.521598360850163</v>
       </c>
       <c r="F34" s="4">
-        <v>0.49210064025115258</v>
+        <v>0.53296588691960423</v>
       </c>
       <c r="G34" s="5">
         <v>1.21455537281616</v>
@@ -2935,19 +3139,19 @@
       <c r="L34" s="4">
         <v>23</v>
       </c>
-      <c r="M34" s="10">
+      <c r="M34" s="9">
         <v>7.4900000000000001E-3</v>
       </c>
       <c r="N34" s="8">
         <v>1.1399999999999999</v>
       </c>
-      <c r="O34" s="10">
+      <c r="O34" s="9">
         <v>3.8530000000000002E-2</v>
       </c>
       <c r="P34" s="8">
         <v>30.23</v>
       </c>
-      <c r="Q34" s="10">
+      <c r="Q34" s="9">
         <v>6.0300000000000006E-3</v>
       </c>
       <c r="R34" s="4">
@@ -2977,14 +3181,15 @@
       <c r="C35" s="8">
         <v>477</v>
       </c>
-      <c r="D35" s="9">
-        <v>0.98397724670378606</v>
+      <c r="D35" s="11">
+        <f>[1]Extraits_Karstnet!H35</f>
+        <v>0.98244681613567253</v>
       </c>
       <c r="E35" s="4">
         <v>330.5110330894214</v>
       </c>
       <c r="F35" s="4">
-        <v>0.3598281907984382</v>
+        <v>0.45813097315895812</v>
       </c>
       <c r="G35" s="5">
         <v>1.5396902592967789</v>
@@ -3004,19 +3209,19 @@
       <c r="L35" s="4">
         <v>4</v>
       </c>
-      <c r="M35" s="10">
+      <c r="M35" s="9">
         <v>3.81E-3</v>
       </c>
       <c r="N35" s="8">
         <v>1.05</v>
       </c>
-      <c r="O35" s="10">
+      <c r="O35" s="9">
         <v>3.6479999999999999E-2</v>
       </c>
       <c r="P35" s="8">
         <v>15.54</v>
       </c>
-      <c r="Q35" s="10">
+      <c r="Q35" s="9">
         <v>3.5600000000000002E-3</v>
       </c>
       <c r="R35" s="4">

</xml_diff>